<commit_message>
fixed the user_page. works now
</commit_message>
<xml_diff>
--- a/data/static/media/VRCNHS_STUDENT_TEMPLATE(CLEAR).xlsx
+++ b/data/static/media/VRCNHS_STUDENT_TEMPLATE(CLEAR).xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gonza\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gonza\Desktop\DEPLOY\vrcnhs-dep-priv\data\static\media\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A989CC6-D7F4-4D42-BB7D-577ED24C8E4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7B5FAC3-1122-411B-B105-D636EA50C356}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="45">
   <si>
     <t>last_name</t>
   </si>
@@ -152,6 +152,9 @@
   </si>
   <si>
     <t>below Php 9,000</t>
+  </si>
+  <si>
+    <t>YYYY-MM-DD</t>
   </si>
 </sst>
 </file>
@@ -327,10 +330,6 @@
   </cellStyles>
   <dxfs count="42">
     <dxf>
-      <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -422,6 +421,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -517,38 +520,38 @@
     <tableColumn id="4" xr3:uid="{29AA9303-1BA1-41F0-AE34-7D1F5D9AC162}" name="middle_name" dataDxfId="34"/>
     <tableColumn id="5" xr3:uid="{29EC0D12-1481-4DA4-B3C1-BC19020DED51}" name="suffix_name" dataDxfId="33"/>
     <tableColumn id="6" xr3:uid="{F1D99430-D426-407A-B2FF-41955249FABB}" name="status" dataDxfId="32"/>
-    <tableColumn id="7" xr3:uid="{2A1DBEDB-763D-4D79-BB1E-5B99DBAEA059}" name="birthday" dataDxfId="0"/>
-    <tableColumn id="8" xr3:uid="{2386CED2-F988-4070-8FEB-FB53F3C31F58}" name="religion" dataDxfId="31"/>
-    <tableColumn id="9" xr3:uid="{79D44F1C-DE2C-4F2B-9A7C-02AA57DF271D}" name="other_religion" dataDxfId="30"/>
-    <tableColumn id="10" xr3:uid="{A9099301-F00D-4393-AAED-580C519A44D6}" name="age" dataDxfId="29"/>
-    <tableColumn id="11" xr3:uid="{0494A6CB-9BF2-4CEE-A382-7E39533947E6}" name="sem" dataDxfId="28"/>
-    <tableColumn id="12" xr3:uid="{054CC827-5E3A-4C91-94D2-ADD89AD45A50}" name="classroom_id" dataDxfId="27"/>
-    <tableColumn id="13" xr3:uid="{C639C3E7-45FC-4090-9433-71C5B914CC2C}" name="gradelevel_id" dataDxfId="26"/>
-    <tableColumn id="14" xr3:uid="{DD29E1BB-A454-41D8-B6B4-B3B0A12A7673}" name="sex" dataDxfId="25"/>
-    <tableColumn id="15" xr3:uid="{C002CDD8-3E6D-4FD3-966C-EA8DD5B38D53}" name="birth_place" dataDxfId="24"/>
-    <tableColumn id="16" xr3:uid="{A29DFC30-9BEA-48E4-B40E-A5432867DC12}" name="mother_tongue" dataDxfId="23"/>
-    <tableColumn id="17" xr3:uid="{3B9F3FFA-3D6E-43AD-A7A5-D8A39F6A7B11}" name="address" dataDxfId="22"/>
-    <tableColumn id="18" xr3:uid="{17BC6193-AD15-4B52-83E8-AFB0756EE442}" name="father_name" dataDxfId="21"/>
-    <tableColumn id="19" xr3:uid="{AFF3B1F9-3D64-4FEB-8A1B-F5502718747B}" name="father_contact" dataDxfId="20"/>
-    <tableColumn id="20" xr3:uid="{703BA395-4DD1-4CC4-B271-18A9028528B5}" name="mother_name" dataDxfId="19"/>
-    <tableColumn id="21" xr3:uid="{D3767B9C-4C9E-4114-A801-D495728A18B6}" name="mother_contact" dataDxfId="18"/>
-    <tableColumn id="22" xr3:uid="{4F4E0722-C99F-4F17-BC55-89EAB7E857C4}" name="guardian_name" dataDxfId="17"/>
-    <tableColumn id="23" xr3:uid="{BEABC783-5F95-47DA-B186-9CC89B11E950}" name="guardian_contact" dataDxfId="16"/>
-    <tableColumn id="24" xr3:uid="{F0414263-D80E-44D9-B53D-3522C4BA5063}" name="last_grade_level" dataDxfId="15"/>
-    <tableColumn id="25" xr3:uid="{0147281F-91DF-4CE4-8B51-52FCF95A7B9E}" name="last_school_attended" dataDxfId="14"/>
-    <tableColumn id="26" xr3:uid="{C6ADF234-7071-4AA9-8F95-E319790EF906}" name="last_schoolyear_completed" dataDxfId="13"/>
-    <tableColumn id="27" xr3:uid="{2BFDCD5E-DC18-4484-8BDD-6BB4A6AE9663}" name="strand" dataDxfId="12"/>
-    <tableColumn id="28" xr3:uid="{B6235BA4-E2C0-42D6-8B96-37913716FE8F}" name="household_income" dataDxfId="11"/>
-    <tableColumn id="29" xr3:uid="{7E4FC1E7-A89D-405F-9D5D-677065FA6C58}" name="is_returnee" dataDxfId="10"/>
-    <tableColumn id="30" xr3:uid="{53E1C59A-4EA4-4B5E-BFF5-9BF65F8F824C}" name="is_a_dropout" dataDxfId="9"/>
-    <tableColumn id="31" xr3:uid="{8013E748-F67D-47F0-B479-C030744C0F84}" name="is_a_working_student" dataDxfId="8"/>
-    <tableColumn id="32" xr3:uid="{1ED14F88-6E4B-49C2-86B9-BD4C18205EB1}" name="previous_adviser" dataDxfId="7"/>
-    <tableColumn id="33" xr3:uid="{FC17A559-CBC0-4AF3-9A4C-0296203ADB23}" name="adviser_contact" dataDxfId="6"/>
-    <tableColumn id="34" xr3:uid="{D580F0C3-7B51-421F-874C-A53019191947}" name="health_bmi" dataDxfId="5"/>
-    <tableColumn id="35" xr3:uid="{BEF3396A-6C86-4F3F-A6F2-1D322EEEE413}" name="general_average" dataDxfId="4"/>
-    <tableColumn id="36" xr3:uid="{38B03E26-8716-459F-8182-4F9B294D5881}" name="is_a_four_ps_scholar" dataDxfId="3"/>
-    <tableColumn id="37" xr3:uid="{0D3DD788-9C77-43B0-9B5C-C7B95DCF988D}" name="edited_fields" dataDxfId="2"/>
-    <tableColumn id="38" xr3:uid="{FEF243F8-A4CB-4855-AF7E-3A6DB8DAFA80}" name="notes" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{2A1DBEDB-763D-4D79-BB1E-5B99DBAEA059}" name="birthday" dataDxfId="31"/>
+    <tableColumn id="8" xr3:uid="{2386CED2-F988-4070-8FEB-FB53F3C31F58}" name="religion" dataDxfId="30"/>
+    <tableColumn id="9" xr3:uid="{79D44F1C-DE2C-4F2B-9A7C-02AA57DF271D}" name="other_religion" dataDxfId="29"/>
+    <tableColumn id="10" xr3:uid="{A9099301-F00D-4393-AAED-580C519A44D6}" name="age" dataDxfId="28"/>
+    <tableColumn id="11" xr3:uid="{0494A6CB-9BF2-4CEE-A382-7E39533947E6}" name="sem" dataDxfId="27"/>
+    <tableColumn id="12" xr3:uid="{054CC827-5E3A-4C91-94D2-ADD89AD45A50}" name="classroom_id" dataDxfId="26"/>
+    <tableColumn id="13" xr3:uid="{C639C3E7-45FC-4090-9433-71C5B914CC2C}" name="gradelevel_id" dataDxfId="25"/>
+    <tableColumn id="14" xr3:uid="{DD29E1BB-A454-41D8-B6B4-B3B0A12A7673}" name="sex" dataDxfId="24"/>
+    <tableColumn id="15" xr3:uid="{C002CDD8-3E6D-4FD3-966C-EA8DD5B38D53}" name="birth_place" dataDxfId="23"/>
+    <tableColumn id="16" xr3:uid="{A29DFC30-9BEA-48E4-B40E-A5432867DC12}" name="mother_tongue" dataDxfId="22"/>
+    <tableColumn id="17" xr3:uid="{3B9F3FFA-3D6E-43AD-A7A5-D8A39F6A7B11}" name="address" dataDxfId="21"/>
+    <tableColumn id="18" xr3:uid="{17BC6193-AD15-4B52-83E8-AFB0756EE442}" name="father_name" dataDxfId="20"/>
+    <tableColumn id="19" xr3:uid="{AFF3B1F9-3D64-4FEB-8A1B-F5502718747B}" name="father_contact" dataDxfId="19"/>
+    <tableColumn id="20" xr3:uid="{703BA395-4DD1-4CC4-B271-18A9028528B5}" name="mother_name" dataDxfId="18"/>
+    <tableColumn id="21" xr3:uid="{D3767B9C-4C9E-4114-A801-D495728A18B6}" name="mother_contact" dataDxfId="17"/>
+    <tableColumn id="22" xr3:uid="{4F4E0722-C99F-4F17-BC55-89EAB7E857C4}" name="guardian_name" dataDxfId="16"/>
+    <tableColumn id="23" xr3:uid="{BEABC783-5F95-47DA-B186-9CC89B11E950}" name="guardian_contact" dataDxfId="15"/>
+    <tableColumn id="24" xr3:uid="{F0414263-D80E-44D9-B53D-3522C4BA5063}" name="last_grade_level" dataDxfId="14"/>
+    <tableColumn id="25" xr3:uid="{0147281F-91DF-4CE4-8B51-52FCF95A7B9E}" name="last_school_attended" dataDxfId="13"/>
+    <tableColumn id="26" xr3:uid="{C6ADF234-7071-4AA9-8F95-E319790EF906}" name="last_schoolyear_completed" dataDxfId="12"/>
+    <tableColumn id="27" xr3:uid="{2BFDCD5E-DC18-4484-8BDD-6BB4A6AE9663}" name="strand" dataDxfId="11"/>
+    <tableColumn id="28" xr3:uid="{B6235BA4-E2C0-42D6-8B96-37913716FE8F}" name="household_income" dataDxfId="10"/>
+    <tableColumn id="29" xr3:uid="{7E4FC1E7-A89D-405F-9D5D-677065FA6C58}" name="is_returnee" dataDxfId="9"/>
+    <tableColumn id="30" xr3:uid="{53E1C59A-4EA4-4B5E-BFF5-9BF65F8F824C}" name="is_a_dropout" dataDxfId="8"/>
+    <tableColumn id="31" xr3:uid="{8013E748-F67D-47F0-B479-C030744C0F84}" name="is_a_working_student" dataDxfId="7"/>
+    <tableColumn id="32" xr3:uid="{1ED14F88-6E4B-49C2-86B9-BD4C18205EB1}" name="previous_adviser" dataDxfId="6"/>
+    <tableColumn id="33" xr3:uid="{FC17A559-CBC0-4AF3-9A4C-0296203ADB23}" name="adviser_contact" dataDxfId="5"/>
+    <tableColumn id="34" xr3:uid="{D580F0C3-7B51-421F-874C-A53019191947}" name="health_bmi" dataDxfId="4"/>
+    <tableColumn id="35" xr3:uid="{BEF3396A-6C86-4F3F-A6F2-1D322EEEE413}" name="general_average" dataDxfId="3"/>
+    <tableColumn id="36" xr3:uid="{38B03E26-8716-459F-8182-4F9B294D5881}" name="is_a_four_ps_scholar" dataDxfId="2"/>
+    <tableColumn id="37" xr3:uid="{0D3DD788-9C77-43B0-9B5C-C7B95DCF988D}" name="edited_fields" dataDxfId="1"/>
+    <tableColumn id="38" xr3:uid="{FEF243F8-A4CB-4855-AF7E-3A6DB8DAFA80}" name="notes" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -844,7 +847,7 @@
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
+      <selection pane="bottomLeft" activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1001,7 +1004,9 @@
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
-      <c r="H2" s="5"/>
+      <c r="H2" s="5" t="s">
+        <v>44</v>
+      </c>
       <c r="I2" s="4"/>
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>

</xml_diff>